<commit_message>
task/ta-167 -- Provide support for lats and longs in the Agent table
top/adp.py
* new methods sanitise_latitude() and sanitise_longitude() (as the
  name says)
* update the sanitise() method to include the lat/long sanitisation
  calls
* update the update() method to include the lat/long sanitisation calls

top/conf/top.conf
* enable the lat and long columns under the [adp_headers] section

top/table/agent.py
* update the agent schema to support new latitude and longitude columns
</commit_message>
<xml_diff>
--- a/top/tests/files/ADP-Bulk-Load-new.xlsx
+++ b/top/tests/files/ADP-Bulk-Load-new.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-1200" yWindow="25720" windowWidth="20480" windowHeight="25160"/>
+    <workbookView xWindow="-320" yWindow="32900" windowWidth="20480" windowHeight="25160"/>
   </bookViews>
   <sheets>
     <sheet name="Export Worksheet" sheetId="1" r:id="rId1"/>
@@ -134,7 +134,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -158,13 +158,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -213,8 +224,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -585,9 +598,9 @@
   </sheetPr>
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
+      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -611,10 +624,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C1" t="s">
@@ -705,6 +718,12 @@
       </c>
       <c r="K2" t="s">
         <v>9</v>
+      </c>
+      <c r="M2" s="2">
+        <v>-35.822864000000003</v>
+      </c>
+      <c r="N2" s="2">
+        <v>155.045278</v>
       </c>
       <c r="O2" t="s">
         <v>10</v>

</xml_diff>